<commit_message>
new vista alegre data
</commit_message>
<xml_diff>
--- a/evaluation/data/evaluation-convergence.xlsx
+++ b/evaluation/data/evaluation-convergence.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tala\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mildo\OneDrive\Documents\R\extension-paitan\evaluation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783D30AC-68E2-4D1B-8CD5-2B15B7F26990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACDD69B-45DB-4861-8846-3FA40E31BA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{87B9E4F4-57DC-404A-AC42-ECBD1809D2CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="264">
   <si>
     <t>name</t>
   </si>
@@ -444,6 +444,390 @@
   </si>
   <si>
     <t>Business/Dressmaking</t>
+  </si>
+  <si>
+    <t>paitan</t>
+  </si>
+  <si>
+    <t>va</t>
+  </si>
+  <si>
+    <t>Handi craft making/urban gardening/food processing</t>
+  </si>
+  <si>
+    <t>Clap 3x  Ang Galing!</t>
+  </si>
+  <si>
+    <t>Vista Alagre BLGU</t>
+  </si>
+  <si>
+    <t>PB</t>
+  </si>
+  <si>
+    <t>Angelo M. Flores</t>
+  </si>
+  <si>
+    <t>Efren S. Molina</t>
+  </si>
+  <si>
+    <t>Glass Cutting</t>
+  </si>
+  <si>
+    <t>Salary/Business</t>
+  </si>
+  <si>
+    <t>15,001-20,000</t>
+  </si>
+  <si>
+    <t>BK</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>Fidel T. Bayatan</t>
+  </si>
+  <si>
+    <t>Carpentry and Mason</t>
+  </si>
+  <si>
+    <t>10,001-15,000</t>
+  </si>
+  <si>
+    <t>John Joan A. Reginalde</t>
+  </si>
+  <si>
+    <t>Jolan A. Paragas</t>
+  </si>
+  <si>
+    <t>Separetad</t>
+  </si>
+  <si>
+    <t>Tanod</t>
+  </si>
+  <si>
+    <t>Gerald A.Bicera</t>
+  </si>
+  <si>
+    <t>plaza</t>
+  </si>
+  <si>
+    <t>Ford Procesing</t>
+  </si>
+  <si>
+    <t>Isinay</t>
+  </si>
+  <si>
+    <t>Crusaders</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Derick R. Eneja</t>
+  </si>
+  <si>
+    <t>Garbage Collector</t>
+  </si>
+  <si>
+    <t>Elynore M. Flores</t>
+  </si>
+  <si>
+    <t>Mushroom production</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>CL/cg</t>
+  </si>
+  <si>
+    <t>Husband carpenter</t>
+  </si>
+  <si>
+    <t>house wife</t>
+  </si>
+  <si>
+    <t>Celestine Grace C. Corpuz</t>
+  </si>
+  <si>
+    <t>Book keeping</t>
+  </si>
+  <si>
+    <t>Congratulation</t>
+  </si>
+  <si>
+    <t>leonardo B. Sandaga</t>
+  </si>
+  <si>
+    <t>Driving</t>
+  </si>
+  <si>
+    <t>Barangay Hall Brgy Vista Alegre</t>
+  </si>
+  <si>
+    <t>brgy treasurer</t>
+  </si>
+  <si>
+    <t>Mary Ann Vicencio</t>
+  </si>
+  <si>
+    <t>Pagtatahi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Josephine S. Sandaga </t>
+  </si>
+  <si>
+    <t>Congratulations! Thank you.</t>
+  </si>
+  <si>
+    <t>More traning on food procesing</t>
+  </si>
+  <si>
+    <t>John L. Catolico</t>
+  </si>
+  <si>
+    <t>Thank you for coming</t>
+  </si>
+  <si>
+    <t>5,001-10,000</t>
+  </si>
+  <si>
+    <t>Brgy employee</t>
+  </si>
+  <si>
+    <t>Brgy Vista Alegre</t>
+  </si>
+  <si>
+    <t>CDN</t>
+  </si>
+  <si>
+    <t>Brgy Honorarium</t>
+  </si>
+  <si>
+    <t>Felix X. Ortiz</t>
+  </si>
+  <si>
+    <t>Vermi Composting</t>
+  </si>
+  <si>
+    <t>Thank you !!</t>
+  </si>
+  <si>
+    <t>Carpentry</t>
+  </si>
+  <si>
+    <t>Jovely C. Balubar</t>
+  </si>
+  <si>
+    <t>Dress Making</t>
+  </si>
+  <si>
+    <t>More traning</t>
+  </si>
+  <si>
+    <t>Fish vendor</t>
+  </si>
+  <si>
+    <t>Tindera</t>
+  </si>
+  <si>
+    <t>Marilyn R.Obana</t>
+  </si>
+  <si>
+    <t>Dress making/Pesteries and Cake</t>
+  </si>
+  <si>
+    <t>Thank you ang more power</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>House  Wife</t>
+  </si>
+  <si>
+    <t>Rosalyn S. Evangelista</t>
+  </si>
+  <si>
+    <t>Bread and Pastry Making</t>
+  </si>
+  <si>
+    <t>Yung time ng sinuman maam dapat mas maaga.Tulong sa part ng participants ang wala sa tamang oras</t>
+  </si>
+  <si>
+    <t>Business/sore owner</t>
+  </si>
+  <si>
+    <t>Flodeln L. Aguirre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dress making </t>
+  </si>
+  <si>
+    <t>More training</t>
+  </si>
+  <si>
+    <t>Brgy Hall Vista Alegre</t>
+  </si>
+  <si>
+    <t>Brgy BHW</t>
+  </si>
+  <si>
+    <t>Carlos O. Ogalde</t>
+  </si>
+  <si>
+    <t>Food Procescing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congratulations </t>
+  </si>
+  <si>
+    <t>Barangay Kagawad</t>
+  </si>
+  <si>
+    <t>Brgy Vista Alegre Bay NV</t>
+  </si>
+  <si>
+    <t>Kagawad</t>
+  </si>
+  <si>
+    <t>Rogelen E. Ramos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dressmaking  </t>
+  </si>
+  <si>
+    <t>More training in Brgy. Vista Alegre</t>
+  </si>
+  <si>
+    <t>Ilocano/Gaddang</t>
+  </si>
+  <si>
+    <t>Brgy Vista Alegre Health Station</t>
+  </si>
+  <si>
+    <t>Melcho R. Buacad</t>
+  </si>
+  <si>
+    <t>Tarala P. Eneja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">va </t>
+  </si>
+  <si>
+    <t>Va</t>
+  </si>
+  <si>
+    <t>Punita L. Lannu</t>
+  </si>
+  <si>
+    <t>Salamat</t>
+  </si>
+  <si>
+    <t>Jobylyn S. Peidad</t>
+  </si>
+  <si>
+    <t>Food processing Traning,Sawing</t>
+  </si>
+  <si>
+    <t>Vista Alegre N.Viz</t>
+  </si>
+  <si>
+    <t>Child development worker</t>
+  </si>
+  <si>
+    <t>Linalyn J. Tejano</t>
+  </si>
+  <si>
+    <t>Visaya</t>
+  </si>
+  <si>
+    <t>Part time</t>
+  </si>
+  <si>
+    <t>Nenita A. Eneja</t>
+  </si>
+  <si>
+    <t>Dress making</t>
+  </si>
+  <si>
+    <t>No comment,Perfect 2xplenation/But more traning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC </t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>Brgy Acetg Clerk</t>
+  </si>
+  <si>
+    <t>BLGU Vista Alegre</t>
+  </si>
+  <si>
+    <t>Brgy Aceonting Clerk</t>
+  </si>
+  <si>
+    <t>Edvalyne G. Valentino</t>
+  </si>
+  <si>
+    <t>Dressmaking</t>
+  </si>
+  <si>
+    <t>Thank you for you advice</t>
+  </si>
+  <si>
+    <t>Home Keeping</t>
+  </si>
+  <si>
+    <t>Norlie M. Capinpin</t>
+  </si>
+  <si>
+    <t>HSl</t>
+  </si>
+  <si>
+    <t>Government/Tanod</t>
+  </si>
+  <si>
+    <t>Vista Alegre Bay. N.Viz</t>
+  </si>
+  <si>
+    <t>Brgy Tanod</t>
+  </si>
+  <si>
+    <t>Edison A. Gulab</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Brgy Vista Alegrex</t>
+  </si>
+  <si>
+    <t>Brgy Tanod electrician</t>
+  </si>
+  <si>
+    <t>Imelda C. Fabian</t>
+  </si>
+  <si>
+    <t>Follow up/Congrats</t>
+  </si>
+  <si>
+    <t>About fsh pond and how to handle</t>
+  </si>
+  <si>
+    <t>Farming/Fishing</t>
   </si>
 </sst>
 </file>
@@ -485,10 +869,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,10 +1211,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7563AC5-D9BA-4BD5-A91C-E7138249B42C}">
-  <dimension ref="A1:AA25"/>
+  <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M5" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,8 +1335,14 @@
       <c r="A2" t="s">
         <v>30</v>
       </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
       <c r="C2" s="1">
         <v>45643</v>
+      </c>
+      <c r="D2" t="s">
+        <v>136</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -1015,8 +1410,14 @@
       <c r="A3" t="s">
         <v>42</v>
       </c>
+      <c r="B3" t="s">
+        <v>136</v>
+      </c>
       <c r="C3" s="1">
         <v>45643</v>
+      </c>
+      <c r="D3" t="s">
+        <v>136</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -1086,8 +1487,14 @@
       <c r="A4" t="s">
         <v>47</v>
       </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
       <c r="C4" s="1">
         <v>45643</v>
+      </c>
+      <c r="D4" t="s">
+        <v>136</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1142,8 +1549,14 @@
       <c r="A5" t="s">
         <v>50</v>
       </c>
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
       <c r="C5" s="1">
         <v>45643</v>
+      </c>
+      <c r="D5" t="s">
+        <v>136</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -1198,8 +1611,14 @@
       <c r="A6" t="s">
         <v>53</v>
       </c>
+      <c r="B6" t="s">
+        <v>136</v>
+      </c>
       <c r="C6" s="1">
         <v>45643</v>
+      </c>
+      <c r="D6" t="s">
+        <v>136</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1260,8 +1679,14 @@
       <c r="A7" t="s">
         <v>59</v>
       </c>
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
       <c r="C7" s="1">
         <v>45643</v>
+      </c>
+      <c r="D7" t="s">
+        <v>136</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -1322,8 +1747,14 @@
       <c r="A8" t="s">
         <v>64</v>
       </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
       <c r="C8" s="1">
         <v>45643</v>
+      </c>
+      <c r="D8" t="s">
+        <v>136</v>
       </c>
       <c r="E8">
         <v>5</v>
@@ -1384,8 +1815,14 @@
       <c r="A9" t="s">
         <v>68</v>
       </c>
+      <c r="B9" t="s">
+        <v>136</v>
+      </c>
       <c r="C9" s="1">
         <v>45643</v>
+      </c>
+      <c r="D9" t="s">
+        <v>136</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -1446,8 +1883,14 @@
       <c r="A10" t="s">
         <v>71</v>
       </c>
+      <c r="B10" t="s">
+        <v>136</v>
+      </c>
       <c r="C10" s="1">
         <v>45643</v>
+      </c>
+      <c r="D10" t="s">
+        <v>136</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -1499,8 +1942,14 @@
       <c r="A11" t="s">
         <v>72</v>
       </c>
+      <c r="B11" t="s">
+        <v>136</v>
+      </c>
       <c r="C11" s="1">
         <v>45643</v>
+      </c>
+      <c r="D11" t="s">
+        <v>136</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -1561,8 +2010,14 @@
       <c r="A12" t="s">
         <v>78</v>
       </c>
+      <c r="B12" t="s">
+        <v>136</v>
+      </c>
       <c r="C12" s="1">
         <v>45643</v>
+      </c>
+      <c r="D12" t="s">
+        <v>136</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -1620,8 +2075,14 @@
       <c r="A13" t="s">
         <v>81</v>
       </c>
+      <c r="B13" t="s">
+        <v>136</v>
+      </c>
       <c r="C13" s="1">
         <v>45643</v>
+      </c>
+      <c r="D13" t="s">
+        <v>136</v>
       </c>
       <c r="E13">
         <v>5</v>
@@ -1679,8 +2140,14 @@
       <c r="A14" t="s">
         <v>84</v>
       </c>
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
       <c r="C14" s="1">
         <v>45643</v>
+      </c>
+      <c r="D14" t="s">
+        <v>136</v>
       </c>
       <c r="E14">
         <v>5</v>
@@ -1732,8 +2199,14 @@
       <c r="A15" t="s">
         <v>88</v>
       </c>
+      <c r="B15" t="s">
+        <v>136</v>
+      </c>
       <c r="C15" s="1">
         <v>45643</v>
+      </c>
+      <c r="D15" t="s">
+        <v>136</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -1785,8 +2258,14 @@
       <c r="A16" t="s">
         <v>92</v>
       </c>
+      <c r="B16" t="s">
+        <v>136</v>
+      </c>
       <c r="C16" s="1">
         <v>45643</v>
+      </c>
+      <c r="D16" t="s">
+        <v>136</v>
       </c>
       <c r="E16">
         <v>5</v>
@@ -1853,8 +2332,14 @@
       <c r="A17" t="s">
         <v>101</v>
       </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
       <c r="C17" s="1">
         <v>45643</v>
+      </c>
+      <c r="D17" t="s">
+        <v>136</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -1912,8 +2397,14 @@
       <c r="A18" t="s">
         <v>102</v>
       </c>
+      <c r="B18" t="s">
+        <v>136</v>
+      </c>
       <c r="C18" s="1">
         <v>45643</v>
+      </c>
+      <c r="D18" t="s">
+        <v>136</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -1971,8 +2462,14 @@
       <c r="A19" t="s">
         <v>105</v>
       </c>
+      <c r="B19" t="s">
+        <v>136</v>
+      </c>
       <c r="C19" s="1">
         <v>45643</v>
+      </c>
+      <c r="D19" t="s">
+        <v>136</v>
       </c>
       <c r="E19">
         <v>5</v>
@@ -2027,8 +2524,14 @@
       <c r="A20" t="s">
         <v>109</v>
       </c>
+      <c r="B20" t="s">
+        <v>136</v>
+      </c>
       <c r="C20" s="1">
         <v>45643</v>
+      </c>
+      <c r="D20" t="s">
+        <v>136</v>
       </c>
       <c r="E20">
         <v>5</v>
@@ -2080,8 +2583,14 @@
       <c r="A21" t="s">
         <v>113</v>
       </c>
+      <c r="B21" t="s">
+        <v>136</v>
+      </c>
       <c r="C21" s="1">
         <v>45643</v>
+      </c>
+      <c r="D21" t="s">
+        <v>136</v>
       </c>
       <c r="E21">
         <v>5</v>
@@ -2145,8 +2654,14 @@
       <c r="A22" t="s">
         <v>119</v>
       </c>
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
       <c r="C22" s="1">
         <v>45643</v>
+      </c>
+      <c r="D22" t="s">
+        <v>136</v>
       </c>
       <c r="E22">
         <v>5</v>
@@ -2216,8 +2731,14 @@
       <c r="A23" t="s">
         <v>125</v>
       </c>
+      <c r="B23" t="s">
+        <v>136</v>
+      </c>
       <c r="C23" s="1">
         <v>45643</v>
+      </c>
+      <c r="D23" t="s">
+        <v>136</v>
       </c>
       <c r="E23">
         <v>5</v>
@@ -2272,8 +2793,14 @@
       <c r="A24" t="s">
         <v>128</v>
       </c>
+      <c r="B24" t="s">
+        <v>136</v>
+      </c>
       <c r="C24" s="1">
         <v>45643</v>
+      </c>
+      <c r="D24" t="s">
+        <v>136</v>
       </c>
       <c r="E24">
         <v>5</v>
@@ -2325,9 +2852,15 @@
       <c r="A25" t="s">
         <v>131</v>
       </c>
+      <c r="B25" t="s">
+        <v>136</v>
+      </c>
       <c r="C25" s="1">
         <v>45643</v>
       </c>
+      <c r="D25" t="s">
+        <v>136</v>
+      </c>
       <c r="E25">
         <v>5</v>
       </c>
@@ -2378,6 +2911,2102 @@
       </c>
       <c r="U25" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>5</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>138</v>
+      </c>
+      <c r="I26" t="s">
+        <v>139</v>
+      </c>
+      <c r="J26" t="s">
+        <v>137</v>
+      </c>
+      <c r="K26" t="s">
+        <v>34</v>
+      </c>
+      <c r="L26" t="s">
+        <v>35</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" t="s">
+        <v>27</v>
+      </c>
+      <c r="O26" s="3">
+        <v>28220</v>
+      </c>
+      <c r="P26">
+        <v>47</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>28</v>
+      </c>
+      <c r="R26" t="s">
+        <v>29</v>
+      </c>
+      <c r="S26" t="s">
+        <v>36</v>
+      </c>
+      <c r="T26" t="s">
+        <v>134</v>
+      </c>
+      <c r="U26" t="s">
+        <v>123</v>
+      </c>
+      <c r="V26" s="4">
+        <v>30000</v>
+      </c>
+      <c r="W26" t="s">
+        <v>39</v>
+      </c>
+      <c r="X26" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>144</v>
+      </c>
+      <c r="J27" t="s">
+        <v>137</v>
+      </c>
+      <c r="K27" t="s">
+        <v>34</v>
+      </c>
+      <c r="L27" t="s">
+        <v>35</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" t="s">
+        <v>27</v>
+      </c>
+      <c r="O27" s="3">
+        <v>28287</v>
+      </c>
+      <c r="P27">
+        <v>47</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>28</v>
+      </c>
+      <c r="R27" t="s">
+        <v>29</v>
+      </c>
+      <c r="S27" t="s">
+        <v>36</v>
+      </c>
+      <c r="T27" t="s">
+        <v>134</v>
+      </c>
+      <c r="U27" t="s">
+        <v>145</v>
+      </c>
+      <c r="V27" t="s">
+        <v>146</v>
+      </c>
+      <c r="W27" t="s">
+        <v>39</v>
+      </c>
+      <c r="X27" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>176</v>
+      </c>
+      <c r="B28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+      <c r="H28" t="s">
+        <v>177</v>
+      </c>
+      <c r="J28" t="s">
+        <v>137</v>
+      </c>
+      <c r="K28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" t="s">
+        <v>35</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" t="s">
+        <v>27</v>
+      </c>
+      <c r="O28" s="5"/>
+      <c r="P28">
+        <v>52</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>28</v>
+      </c>
+      <c r="R28" t="s">
+        <v>29</v>
+      </c>
+      <c r="S28" t="s">
+        <v>148</v>
+      </c>
+      <c r="T28" t="s">
+        <v>58</v>
+      </c>
+      <c r="V28" t="s">
+        <v>146</v>
+      </c>
+      <c r="W28" t="s">
+        <v>39</v>
+      </c>
+      <c r="X28" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>149</v>
+      </c>
+      <c r="B29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D29" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29" t="s">
+        <v>150</v>
+      </c>
+      <c r="J29" t="s">
+        <v>137</v>
+      </c>
+      <c r="K29" t="s">
+        <v>34</v>
+      </c>
+      <c r="L29" t="s">
+        <v>35</v>
+      </c>
+      <c r="M29">
+        <v>9677151666</v>
+      </c>
+      <c r="N29" t="s">
+        <v>27</v>
+      </c>
+      <c r="O29" s="3">
+        <v>25236</v>
+      </c>
+      <c r="P29">
+        <v>56</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>28</v>
+      </c>
+      <c r="R29" t="s">
+        <v>108</v>
+      </c>
+      <c r="S29" t="s">
+        <v>116</v>
+      </c>
+      <c r="T29" t="s">
+        <v>37</v>
+      </c>
+      <c r="U29" t="s">
+        <v>123</v>
+      </c>
+      <c r="V29" t="s">
+        <v>151</v>
+      </c>
+      <c r="W29" t="s">
+        <v>39</v>
+      </c>
+      <c r="X29" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D30" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" t="s">
+        <v>150</v>
+      </c>
+      <c r="J30" t="s">
+        <v>137</v>
+      </c>
+      <c r="K30" t="s">
+        <v>34</v>
+      </c>
+      <c r="L30" t="s">
+        <v>35</v>
+      </c>
+      <c r="M30">
+        <v>9565612415</v>
+      </c>
+      <c r="N30" t="s">
+        <v>27</v>
+      </c>
+      <c r="O30" s="3">
+        <v>25640</v>
+      </c>
+      <c r="P30">
+        <v>54</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>28</v>
+      </c>
+      <c r="R30" t="s">
+        <v>29</v>
+      </c>
+      <c r="S30" t="s">
+        <v>36</v>
+      </c>
+      <c r="T30" t="s">
+        <v>58</v>
+      </c>
+      <c r="U30" t="s">
+        <v>123</v>
+      </c>
+      <c r="V30" t="s">
+        <v>151</v>
+      </c>
+      <c r="W30" t="s">
+        <v>39</v>
+      </c>
+      <c r="X30" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D31" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31">
+        <v>4</v>
+      </c>
+      <c r="J31" t="s">
+        <v>137</v>
+      </c>
+      <c r="K31" t="s">
+        <v>34</v>
+      </c>
+      <c r="L31" t="s">
+        <v>35</v>
+      </c>
+      <c r="M31">
+        <v>9554914776</v>
+      </c>
+      <c r="N31" t="s">
+        <v>27</v>
+      </c>
+      <c r="O31" s="3">
+        <v>30665</v>
+      </c>
+      <c r="P31">
+        <v>41</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>154</v>
+      </c>
+      <c r="S31" t="s">
+        <v>36</v>
+      </c>
+      <c r="T31" t="s">
+        <v>134</v>
+      </c>
+      <c r="U31" t="s">
+        <v>123</v>
+      </c>
+      <c r="W31" t="s">
+        <v>155</v>
+      </c>
+      <c r="X31" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D32" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32">
+        <v>4</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32" t="s">
+        <v>158</v>
+      </c>
+      <c r="J32" t="s">
+        <v>137</v>
+      </c>
+      <c r="K32" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" t="s">
+        <v>35</v>
+      </c>
+      <c r="M32">
+        <v>9355364181</v>
+      </c>
+      <c r="N32" t="s">
+        <v>27</v>
+      </c>
+      <c r="O32" s="3">
+        <v>28736</v>
+      </c>
+      <c r="P32">
+        <v>46</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>28</v>
+      </c>
+      <c r="R32" t="s">
+        <v>159</v>
+      </c>
+      <c r="S32" t="s">
+        <v>160</v>
+      </c>
+      <c r="T32" t="s">
+        <v>161</v>
+      </c>
+      <c r="U32" t="s">
+        <v>123</v>
+      </c>
+      <c r="V32" s="4">
+        <v>5000</v>
+      </c>
+      <c r="W32" t="s">
+        <v>39</v>
+      </c>
+      <c r="X32" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D33" t="s">
+        <v>137</v>
+      </c>
+      <c r="E33">
+        <v>5</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="J33" t="s">
+        <v>137</v>
+      </c>
+      <c r="K33" t="s">
+        <v>34</v>
+      </c>
+      <c r="L33" t="s">
+        <v>35</v>
+      </c>
+      <c r="O33" s="3">
+        <v>24723</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>28</v>
+      </c>
+      <c r="R33" t="s">
+        <v>29</v>
+      </c>
+      <c r="S33" t="s">
+        <v>29</v>
+      </c>
+      <c r="T33" t="s">
+        <v>163</v>
+      </c>
+      <c r="U33" t="s">
+        <v>117</v>
+      </c>
+      <c r="V33" s="4">
+        <v>5000</v>
+      </c>
+      <c r="W33" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D34" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+      <c r="J34" t="s">
+        <v>137</v>
+      </c>
+      <c r="K34" t="s">
+        <v>34</v>
+      </c>
+      <c r="L34" t="s">
+        <v>35</v>
+      </c>
+      <c r="N34" t="s">
+        <v>27</v>
+      </c>
+      <c r="O34" s="3">
+        <v>36985</v>
+      </c>
+      <c r="P34">
+        <v>23</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>86</v>
+      </c>
+      <c r="R34" t="s">
+        <v>108</v>
+      </c>
+      <c r="S34" t="s">
+        <v>36</v>
+      </c>
+      <c r="T34" t="s">
+        <v>77</v>
+      </c>
+      <c r="X34" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>167</v>
+      </c>
+      <c r="B35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D35" t="s">
+        <v>137</v>
+      </c>
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35" t="s">
+        <v>168</v>
+      </c>
+      <c r="I35" t="s">
+        <v>169</v>
+      </c>
+      <c r="J35" t="s">
+        <v>137</v>
+      </c>
+      <c r="K35" t="s">
+        <v>34</v>
+      </c>
+      <c r="M35">
+        <v>9753307481</v>
+      </c>
+      <c r="N35" t="s">
+        <v>49</v>
+      </c>
+      <c r="O35" s="3">
+        <v>27016</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>28</v>
+      </c>
+      <c r="R35" t="s">
+        <v>29</v>
+      </c>
+      <c r="S35" t="s">
+        <v>36</v>
+      </c>
+      <c r="T35" t="s">
+        <v>170</v>
+      </c>
+      <c r="U35" t="s">
+        <v>171</v>
+      </c>
+      <c r="V35" s="4">
+        <v>5000</v>
+      </c>
+      <c r="W35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" t="s">
+        <v>137</v>
+      </c>
+      <c r="C36" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36">
+        <v>5</v>
+      </c>
+      <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="G36">
+        <v>5</v>
+      </c>
+      <c r="H36" t="s">
+        <v>174</v>
+      </c>
+      <c r="I36" t="s">
+        <v>175</v>
+      </c>
+      <c r="J36" t="s">
+        <v>137</v>
+      </c>
+      <c r="K36" t="s">
+        <v>34</v>
+      </c>
+      <c r="L36" t="s">
+        <v>35</v>
+      </c>
+      <c r="M36">
+        <v>9168390003</v>
+      </c>
+      <c r="N36" t="s">
+        <v>49</v>
+      </c>
+      <c r="O36" s="3">
+        <v>30454</v>
+      </c>
+      <c r="P36">
+        <v>41</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>28</v>
+      </c>
+      <c r="R36" t="s">
+        <v>29</v>
+      </c>
+      <c r="S36" t="s">
+        <v>90</v>
+      </c>
+      <c r="T36" t="s">
+        <v>58</v>
+      </c>
+      <c r="U36" t="s">
+        <v>123</v>
+      </c>
+      <c r="V36" t="s">
+        <v>146</v>
+      </c>
+      <c r="W36" t="s">
+        <v>39</v>
+      </c>
+      <c r="X36" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D37" t="s">
+        <v>137</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>5</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37" t="s">
+        <v>181</v>
+      </c>
+      <c r="J37" t="s">
+        <v>137</v>
+      </c>
+      <c r="K37" t="s">
+        <v>34</v>
+      </c>
+      <c r="L37" t="s">
+        <v>35</v>
+      </c>
+      <c r="O37" s="3">
+        <v>24723</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>28</v>
+      </c>
+      <c r="R37" t="s">
+        <v>29</v>
+      </c>
+      <c r="S37" t="s">
+        <v>36</v>
+      </c>
+      <c r="T37" t="s">
+        <v>163</v>
+      </c>
+      <c r="V37" s="4">
+        <v>5000</v>
+      </c>
+      <c r="W37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>182</v>
+      </c>
+      <c r="B38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38" t="s">
+        <v>184</v>
+      </c>
+      <c r="I38" t="s">
+        <v>183</v>
+      </c>
+      <c r="J38" t="s">
+        <v>137</v>
+      </c>
+      <c r="K38" t="s">
+        <v>34</v>
+      </c>
+      <c r="L38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M38">
+        <v>9655517462</v>
+      </c>
+      <c r="N38" t="s">
+        <v>49</v>
+      </c>
+      <c r="O38" s="3">
+        <v>23223</v>
+      </c>
+      <c r="P38">
+        <v>61</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>76</v>
+      </c>
+      <c r="R38" t="s">
+        <v>29</v>
+      </c>
+      <c r="S38" t="s">
+        <v>36</v>
+      </c>
+      <c r="T38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>185</v>
+      </c>
+      <c r="B39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D39" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
+      <c r="H39" t="s">
+        <v>158</v>
+      </c>
+      <c r="I39" t="s">
+        <v>186</v>
+      </c>
+      <c r="J39" t="s">
+        <v>137</v>
+      </c>
+      <c r="K39" t="s">
+        <v>34</v>
+      </c>
+      <c r="L39" t="s">
+        <v>35</v>
+      </c>
+      <c r="M39">
+        <v>9558916105</v>
+      </c>
+      <c r="N39" t="s">
+        <v>27</v>
+      </c>
+      <c r="O39" s="3">
+        <v>28280</v>
+      </c>
+      <c r="P39">
+        <v>48</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>28</v>
+      </c>
+      <c r="R39" t="s">
+        <v>29</v>
+      </c>
+      <c r="S39" t="s">
+        <v>36</v>
+      </c>
+      <c r="T39" t="s">
+        <v>58</v>
+      </c>
+      <c r="U39" t="s">
+        <v>191</v>
+      </c>
+      <c r="V39" t="s">
+        <v>187</v>
+      </c>
+      <c r="W39" t="s">
+        <v>188</v>
+      </c>
+      <c r="X39" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>192</v>
+      </c>
+      <c r="B40" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D40" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40">
+        <v>5</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="H40" t="s">
+        <v>193</v>
+      </c>
+      <c r="I40" t="s">
+        <v>194</v>
+      </c>
+      <c r="J40" t="s">
+        <v>137</v>
+      </c>
+      <c r="K40" t="s">
+        <v>34</v>
+      </c>
+      <c r="L40" t="s">
+        <v>35</v>
+      </c>
+      <c r="N40" t="s">
+        <v>27</v>
+      </c>
+      <c r="O40" s="3">
+        <v>20219</v>
+      </c>
+      <c r="P40">
+        <v>70</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>76</v>
+      </c>
+      <c r="R40" t="s">
+        <v>108</v>
+      </c>
+      <c r="S40" t="s">
+        <v>36</v>
+      </c>
+      <c r="T40" t="s">
+        <v>63</v>
+      </c>
+      <c r="U40" t="s">
+        <v>195</v>
+      </c>
+      <c r="V40" s="4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>196</v>
+      </c>
+      <c r="B41" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D41" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>5</v>
+      </c>
+      <c r="G41">
+        <v>5</v>
+      </c>
+      <c r="H41" t="s">
+        <v>197</v>
+      </c>
+      <c r="I41" t="s">
+        <v>198</v>
+      </c>
+      <c r="J41" t="s">
+        <v>137</v>
+      </c>
+      <c r="K41" t="s">
+        <v>34</v>
+      </c>
+      <c r="L41" t="s">
+        <v>35</v>
+      </c>
+      <c r="N41" t="s">
+        <v>49</v>
+      </c>
+      <c r="O41" s="3">
+        <v>31938</v>
+      </c>
+      <c r="P41">
+        <v>38</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>28</v>
+      </c>
+      <c r="R41" t="s">
+        <v>29</v>
+      </c>
+      <c r="S41" t="s">
+        <v>36</v>
+      </c>
+      <c r="T41" t="s">
+        <v>112</v>
+      </c>
+      <c r="U41" t="s">
+        <v>199</v>
+      </c>
+      <c r="V41" s="4">
+        <v>5000</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>201</v>
+      </c>
+      <c r="B42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" t="s">
+        <v>137</v>
+      </c>
+      <c r="E42">
+        <v>5</v>
+      </c>
+      <c r="F42">
+        <v>5</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+      <c r="H42" t="s">
+        <v>202</v>
+      </c>
+      <c r="I42" t="s">
+        <v>203</v>
+      </c>
+      <c r="J42" t="s">
+        <v>137</v>
+      </c>
+      <c r="K42" t="s">
+        <v>34</v>
+      </c>
+      <c r="L42" t="s">
+        <v>35</v>
+      </c>
+      <c r="M42">
+        <v>9358551814</v>
+      </c>
+      <c r="N42" t="s">
+        <v>49</v>
+      </c>
+      <c r="O42" s="3">
+        <v>26391</v>
+      </c>
+      <c r="P42">
+        <v>51</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>28</v>
+      </c>
+      <c r="R42" t="s">
+        <v>29</v>
+      </c>
+      <c r="S42" t="s">
+        <v>36</v>
+      </c>
+      <c r="T42" t="s">
+        <v>37</v>
+      </c>
+      <c r="U42" t="s">
+        <v>204</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>206</v>
+      </c>
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43">
+        <v>5</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43">
+        <v>5</v>
+      </c>
+      <c r="H43" t="s">
+        <v>207</v>
+      </c>
+      <c r="I43" t="s">
+        <v>208</v>
+      </c>
+      <c r="J43" t="s">
+        <v>137</v>
+      </c>
+      <c r="K43" t="s">
+        <v>34</v>
+      </c>
+      <c r="L43" t="s">
+        <v>35</v>
+      </c>
+      <c r="M43">
+        <v>9161740570</v>
+      </c>
+      <c r="N43" t="s">
+        <v>49</v>
+      </c>
+      <c r="O43" s="3">
+        <v>29763</v>
+      </c>
+      <c r="P43">
+        <v>43</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>28</v>
+      </c>
+      <c r="R43" t="s">
+        <v>29</v>
+      </c>
+      <c r="S43" t="s">
+        <v>111</v>
+      </c>
+      <c r="T43" t="s">
+        <v>134</v>
+      </c>
+      <c r="U43" t="s">
+        <v>209</v>
+      </c>
+      <c r="V43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>210</v>
+      </c>
+      <c r="B44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D44" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44">
+        <v>5</v>
+      </c>
+      <c r="F44">
+        <v>5</v>
+      </c>
+      <c r="G44">
+        <v>5</v>
+      </c>
+      <c r="H44" t="s">
+        <v>211</v>
+      </c>
+      <c r="I44" t="s">
+        <v>212</v>
+      </c>
+      <c r="J44" t="s">
+        <v>137</v>
+      </c>
+      <c r="K44" t="s">
+        <v>34</v>
+      </c>
+      <c r="L44" t="s">
+        <v>35</v>
+      </c>
+      <c r="M44">
+        <v>9753238780</v>
+      </c>
+      <c r="N44" t="s">
+        <v>49</v>
+      </c>
+      <c r="O44" s="3">
+        <v>31613</v>
+      </c>
+      <c r="P44">
+        <v>38</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>28</v>
+      </c>
+      <c r="R44" t="s">
+        <v>95</v>
+      </c>
+      <c r="S44" t="s">
+        <v>36</v>
+      </c>
+      <c r="T44" t="s">
+        <v>58</v>
+      </c>
+      <c r="U44" t="s">
+        <v>123</v>
+      </c>
+      <c r="V44" s="4">
+        <v>3750</v>
+      </c>
+      <c r="W44" t="s">
+        <v>39</v>
+      </c>
+      <c r="X44" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>215</v>
+      </c>
+      <c r="B45" t="s">
+        <v>137</v>
+      </c>
+      <c r="C45" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D45" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="G45">
+        <v>5</v>
+      </c>
+      <c r="H45" t="s">
+        <v>216</v>
+      </c>
+      <c r="I45" t="s">
+        <v>217</v>
+      </c>
+      <c r="J45" t="s">
+        <v>137</v>
+      </c>
+      <c r="K45" t="s">
+        <v>34</v>
+      </c>
+      <c r="L45" t="s">
+        <v>35</v>
+      </c>
+      <c r="M45">
+        <v>9525723476</v>
+      </c>
+      <c r="N45" t="s">
+        <v>27</v>
+      </c>
+      <c r="O45" s="3">
+        <v>17840</v>
+      </c>
+      <c r="P45">
+        <v>76</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>28</v>
+      </c>
+      <c r="R45" t="s">
+        <v>29</v>
+      </c>
+      <c r="S45" t="s">
+        <v>36</v>
+      </c>
+      <c r="T45" t="s">
+        <v>134</v>
+      </c>
+      <c r="U45" t="s">
+        <v>218</v>
+      </c>
+      <c r="V45" t="s">
+        <v>146</v>
+      </c>
+      <c r="W45" t="s">
+        <v>39</v>
+      </c>
+      <c r="X45" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>221</v>
+      </c>
+      <c r="B46" t="s">
+        <v>137</v>
+      </c>
+      <c r="C46" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D46" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>5</v>
+      </c>
+      <c r="G46">
+        <v>5</v>
+      </c>
+      <c r="H46" t="s">
+        <v>222</v>
+      </c>
+      <c r="I46" t="s">
+        <v>223</v>
+      </c>
+      <c r="J46" t="s">
+        <v>137</v>
+      </c>
+      <c r="K46" t="s">
+        <v>34</v>
+      </c>
+      <c r="L46" t="s">
+        <v>35</v>
+      </c>
+      <c r="M46">
+        <v>9676775379</v>
+      </c>
+      <c r="N46" t="s">
+        <v>49</v>
+      </c>
+      <c r="O46" s="3">
+        <v>27938</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>86</v>
+      </c>
+      <c r="R46" t="s">
+        <v>224</v>
+      </c>
+      <c r="S46" t="s">
+        <v>116</v>
+      </c>
+      <c r="T46" t="s">
+        <v>77</v>
+      </c>
+      <c r="U46" t="s">
+        <v>123</v>
+      </c>
+      <c r="V46" s="4">
+        <v>3750</v>
+      </c>
+      <c r="W46" t="s">
+        <v>46</v>
+      </c>
+      <c r="X46" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D47" t="s">
+        <v>137</v>
+      </c>
+      <c r="J47" t="s">
+        <v>137</v>
+      </c>
+      <c r="K47" t="s">
+        <v>34</v>
+      </c>
+      <c r="L47" t="s">
+        <v>35</v>
+      </c>
+      <c r="N47" t="s">
+        <v>27</v>
+      </c>
+      <c r="O47" s="3">
+        <v>22431</v>
+      </c>
+      <c r="P47">
+        <v>63</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>28</v>
+      </c>
+      <c r="R47" t="s">
+        <v>29</v>
+      </c>
+      <c r="S47" t="s">
+        <v>36</v>
+      </c>
+      <c r="T47" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>227</v>
+      </c>
+      <c r="B48" t="s">
+        <v>228</v>
+      </c>
+      <c r="C48" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D48" t="s">
+        <v>137</v>
+      </c>
+      <c r="E48">
+        <v>5</v>
+      </c>
+      <c r="F48">
+        <v>5</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="J48" t="s">
+        <v>229</v>
+      </c>
+      <c r="K48" t="s">
+        <v>34</v>
+      </c>
+      <c r="L48" t="s">
+        <v>35</v>
+      </c>
+      <c r="O48" s="3">
+        <v>23688</v>
+      </c>
+      <c r="P48">
+        <v>60</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>154</v>
+      </c>
+      <c r="R48" t="s">
+        <v>29</v>
+      </c>
+      <c r="S48" t="s">
+        <v>36</v>
+      </c>
+      <c r="T48" t="s">
+        <v>37</v>
+      </c>
+      <c r="U48" t="s">
+        <v>123</v>
+      </c>
+      <c r="V48" s="4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>230</v>
+      </c>
+      <c r="B49" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D49" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49">
+        <v>5</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49" t="s">
+        <v>168</v>
+      </c>
+      <c r="I49" t="s">
+        <v>231</v>
+      </c>
+      <c r="J49" t="s">
+        <v>137</v>
+      </c>
+      <c r="K49" t="s">
+        <v>34</v>
+      </c>
+      <c r="L49" t="s">
+        <v>35</v>
+      </c>
+      <c r="M49">
+        <v>9055893100</v>
+      </c>
+      <c r="N49" t="s">
+        <v>49</v>
+      </c>
+      <c r="O49" s="3">
+        <v>23708</v>
+      </c>
+      <c r="P49">
+        <v>60</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>76</v>
+      </c>
+      <c r="R49" t="s">
+        <v>95</v>
+      </c>
+      <c r="S49" t="s">
+        <v>36</v>
+      </c>
+      <c r="T49" t="s">
+        <v>58</v>
+      </c>
+      <c r="U49" t="s">
+        <v>123</v>
+      </c>
+      <c r="V49" s="4">
+        <v>5000</v>
+      </c>
+      <c r="W49" t="s">
+        <v>39</v>
+      </c>
+      <c r="X49" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>232</v>
+      </c>
+      <c r="B50" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D50" t="s">
+        <v>137</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
+      <c r="F50">
+        <v>4</v>
+      </c>
+      <c r="G50">
+        <v>4</v>
+      </c>
+      <c r="H50" t="s">
+        <v>233</v>
+      </c>
+      <c r="J50" t="s">
+        <v>137</v>
+      </c>
+      <c r="K50" t="s">
+        <v>34</v>
+      </c>
+      <c r="L50" t="s">
+        <v>35</v>
+      </c>
+      <c r="M50">
+        <v>9152126185</v>
+      </c>
+      <c r="N50" t="s">
+        <v>49</v>
+      </c>
+      <c r="O50" s="3">
+        <v>29238</v>
+      </c>
+      <c r="P50">
+        <v>45</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>28</v>
+      </c>
+      <c r="S50" t="s">
+        <v>36</v>
+      </c>
+      <c r="T50" t="s">
+        <v>58</v>
+      </c>
+      <c r="U50" t="s">
+        <v>123</v>
+      </c>
+      <c r="V50" s="6">
+        <v>4850.1000000000004</v>
+      </c>
+      <c r="W50" t="s">
+        <v>39</v>
+      </c>
+      <c r="X50" t="s">
+        <v>234</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>236</v>
+      </c>
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D51" t="s">
+        <v>137</v>
+      </c>
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51">
+        <v>5</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51" t="s">
+        <v>181</v>
+      </c>
+      <c r="J51" t="s">
+        <v>137</v>
+      </c>
+      <c r="K51" t="s">
+        <v>34</v>
+      </c>
+      <c r="L51" t="s">
+        <v>35</v>
+      </c>
+      <c r="M51">
+        <v>9358661256</v>
+      </c>
+      <c r="O51" s="3">
+        <v>25947</v>
+      </c>
+      <c r="P51">
+        <v>54</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>86</v>
+      </c>
+      <c r="R51" t="s">
+        <v>237</v>
+      </c>
+      <c r="S51" t="s">
+        <v>36</v>
+      </c>
+      <c r="T51" t="s">
+        <v>112</v>
+      </c>
+      <c r="U51" t="s">
+        <v>238</v>
+      </c>
+      <c r="V51" s="4">
+        <v>5000</v>
+      </c>
+      <c r="W51" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>239</v>
+      </c>
+      <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D52" t="s">
+        <v>137</v>
+      </c>
+      <c r="E52">
+        <v>5</v>
+      </c>
+      <c r="F52">
+        <v>5</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+      <c r="H52" t="s">
+        <v>240</v>
+      </c>
+      <c r="I52" t="s">
+        <v>241</v>
+      </c>
+      <c r="J52" t="s">
+        <v>228</v>
+      </c>
+      <c r="K52" t="s">
+        <v>34</v>
+      </c>
+      <c r="L52" t="s">
+        <v>35</v>
+      </c>
+      <c r="M52">
+        <v>9555494607</v>
+      </c>
+      <c r="N52" t="s">
+        <v>49</v>
+      </c>
+      <c r="O52" s="3">
+        <v>18972</v>
+      </c>
+      <c r="P52">
+        <v>74</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>76</v>
+      </c>
+      <c r="R52" t="s">
+        <v>108</v>
+      </c>
+      <c r="S52" t="s">
+        <v>242</v>
+      </c>
+      <c r="T52" t="s">
+        <v>243</v>
+      </c>
+      <c r="U52" t="s">
+        <v>244</v>
+      </c>
+      <c r="V52" s="4">
+        <v>5000</v>
+      </c>
+      <c r="W52" t="s">
+        <v>39</v>
+      </c>
+      <c r="X52" t="s">
+        <v>245</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>247</v>
+      </c>
+      <c r="B53" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D53" t="s">
+        <v>137</v>
+      </c>
+      <c r="E53">
+        <v>5</v>
+      </c>
+      <c r="F53">
+        <v>5</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53" t="s">
+        <v>248</v>
+      </c>
+      <c r="I53" t="s">
+        <v>249</v>
+      </c>
+      <c r="J53" t="s">
+        <v>137</v>
+      </c>
+      <c r="K53" t="s">
+        <v>34</v>
+      </c>
+      <c r="L53" t="s">
+        <v>35</v>
+      </c>
+      <c r="M53">
+        <v>9058136835</v>
+      </c>
+      <c r="N53" t="s">
+        <v>49</v>
+      </c>
+      <c r="O53" s="3">
+        <v>20088</v>
+      </c>
+      <c r="P53">
+        <v>70</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>76</v>
+      </c>
+      <c r="S53" t="s">
+        <v>36</v>
+      </c>
+      <c r="T53" t="s">
+        <v>134</v>
+      </c>
+      <c r="U53" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>251</v>
+      </c>
+      <c r="B54" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="3">
+        <v>42054</v>
+      </c>
+      <c r="D54" t="s">
+        <v>137</v>
+      </c>
+      <c r="E54">
+        <v>5</v>
+      </c>
+      <c r="F54">
+        <v>5</v>
+      </c>
+      <c r="G54">
+        <v>5</v>
+      </c>
+      <c r="H54" t="s">
+        <v>158</v>
+      </c>
+      <c r="J54" t="s">
+        <v>137</v>
+      </c>
+      <c r="K54" t="s">
+        <v>34</v>
+      </c>
+      <c r="L54" t="s">
+        <v>35</v>
+      </c>
+      <c r="M54">
+        <v>9753303417</v>
+      </c>
+      <c r="N54" t="s">
+        <v>27</v>
+      </c>
+      <c r="O54" s="3">
+        <v>25512</v>
+      </c>
+      <c r="P54">
+        <v>55</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>28</v>
+      </c>
+      <c r="R54" t="s">
+        <v>29</v>
+      </c>
+      <c r="S54" t="s">
+        <v>36</v>
+      </c>
+      <c r="T54" t="s">
+        <v>252</v>
+      </c>
+      <c r="U54" t="s">
+        <v>123</v>
+      </c>
+      <c r="W54" t="s">
+        <v>253</v>
+      </c>
+      <c r="X54" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>256</v>
+      </c>
+      <c r="B55" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D55" t="s">
+        <v>137</v>
+      </c>
+      <c r="E55">
+        <v>5</v>
+      </c>
+      <c r="F55">
+        <v>5</v>
+      </c>
+      <c r="G55">
+        <v>5</v>
+      </c>
+      <c r="J55" t="s">
+        <v>228</v>
+      </c>
+      <c r="K55" t="s">
+        <v>34</v>
+      </c>
+      <c r="L55" t="s">
+        <v>35</v>
+      </c>
+      <c r="M55">
+        <v>9307155279</v>
+      </c>
+      <c r="N55" t="s">
+        <v>27</v>
+      </c>
+      <c r="O55" s="3">
+        <v>28369</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>28</v>
+      </c>
+      <c r="R55" t="s">
+        <v>224</v>
+      </c>
+      <c r="S55" t="s">
+        <v>36</v>
+      </c>
+      <c r="T55" t="s">
+        <v>37</v>
+      </c>
+      <c r="V55" s="4">
+        <v>3000</v>
+      </c>
+      <c r="W55" t="s">
+        <v>257</v>
+      </c>
+      <c r="X55" t="s">
+        <v>258</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>260</v>
+      </c>
+      <c r="B56" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" s="3">
+        <v>45707</v>
+      </c>
+      <c r="D56" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56">
+        <v>5</v>
+      </c>
+      <c r="F56">
+        <v>5</v>
+      </c>
+      <c r="G56">
+        <v>4</v>
+      </c>
+      <c r="H56" t="s">
+        <v>262</v>
+      </c>
+      <c r="I56" t="s">
+        <v>261</v>
+      </c>
+      <c r="J56" t="s">
+        <v>137</v>
+      </c>
+      <c r="K56" t="s">
+        <v>34</v>
+      </c>
+      <c r="L56" t="s">
+        <v>35</v>
+      </c>
+      <c r="M56">
+        <v>9555493808</v>
+      </c>
+      <c r="N56" t="s">
+        <v>49</v>
+      </c>
+      <c r="O56" s="3">
+        <v>22079</v>
+      </c>
+      <c r="P56">
+        <v>64</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>28</v>
+      </c>
+      <c r="R56" t="s">
+        <v>95</v>
+      </c>
+      <c r="S56" t="s">
+        <v>36</v>
+      </c>
+      <c r="T56" t="s">
+        <v>58</v>
+      </c>
+      <c r="U56" t="s">
+        <v>263</v>
+      </c>
+      <c r="V56" s="4">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>